<commit_message>
redone results with farm productivity growth
</commit_message>
<xml_diff>
--- a/Outputs/Summary Stats.xlsx
+++ b/Outputs/Summary Stats.xlsx
@@ -97,13 +97,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>1.6423550416685369E7</v>
+        <v>4.298652703819948E7</v>
       </c>
       <c r="C2" t="n">
-        <v>2.605998431199456E7</v>
+        <v>5.984996484684038E7</v>
       </c>
       <c r="D2" t="n">
-        <v>1.4505592921025458E8</v>
+        <v>2.6461698829282954E8</v>
       </c>
     </row>
     <row r="3">
@@ -111,13 +111,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>5.026514105865126E7</v>
+        <v>5.035768338647374E7</v>
       </c>
       <c r="C3" t="n">
-        <v>4.8870950662555844E8</v>
+        <v>4.9209284847966754E8</v>
       </c>
       <c r="D3" t="n">
-        <v>9.459334194265753E9</v>
+        <v>1.4197923632578537E10</v>
       </c>
     </row>
     <row r="4">
@@ -125,13 +125,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>1.5087791270884416E8</v>
+        <v>1.1889642435539998E8</v>
       </c>
       <c r="C4" t="n">
-        <v>3.2250041251117253E8</v>
+        <v>3.0091602142223704E8</v>
       </c>
       <c r="D4" t="n">
-        <v>4.2759883316715384E9</v>
+        <v>6.548654199625336E9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>